<commit_message>
Working checkpoint (data viewer)
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/NatureProps/inputs/field and function mapping tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F169695-AC73-4CEF-A20D-2171419F30B4}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1D7D66E-81D7-4046-81DA-CBB16616D891}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="161">
   <si>
     <t>db_name</t>
   </si>
@@ -402,6 +402,120 @@
   </si>
   <si>
     <t>pid_view_03</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>landowner_contact_details</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>name_last</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>name_first</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email </t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Home Phone</t>
+  </si>
+  <si>
+    <t>phone_home</t>
+  </si>
+  <si>
+    <t>Cell Phone</t>
+  </si>
+  <si>
+    <t>phone_cell</t>
+  </si>
+  <si>
+    <t>Landowner PIDs</t>
+  </si>
+  <si>
+    <t>landowner_pids</t>
+  </si>
+  <si>
+    <t>DNC</t>
+  </si>
+  <si>
+    <t>dnc</t>
+  </si>
+  <si>
+    <t>landowner_communication</t>
+  </si>
+  <si>
+    <t>Landowner Contact ID</t>
+  </si>
+  <si>
+    <t>landowner_contact_id</t>
+  </si>
+  <si>
+    <t>Communication Purpose</t>
+  </si>
+  <si>
+    <t>communication_purpose_id</t>
+  </si>
+  <si>
+    <t>Communication Method</t>
+  </si>
+  <si>
+    <t>communication_method_id</t>
+  </si>
+  <si>
+    <t>Date Contacted</t>
+  </si>
+  <si>
+    <t>date_contacted</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>communication_description</t>
+  </si>
+  <si>
+    <t>Date Follow Up</t>
+  </si>
+  <si>
+    <t>date_follow_up</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>parcels</t>
+  </si>
+  <si>
+    <t>communication_purpose</t>
+  </si>
+  <si>
+    <t>communication_method</t>
+  </si>
+  <si>
+    <t>method_value</t>
+  </si>
+  <si>
+    <t>purpose_value</t>
+  </si>
+  <si>
+    <t>communication_purpose_value</t>
+  </si>
+  <si>
+    <t>communication_method_value</t>
+  </si>
+  <si>
+    <t>communication_data_view</t>
   </si>
 </sst>
 </file>
@@ -1251,28 +1365,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.69921875" customWidth="1"/>
-    <col min="4" max="4" width="8.59765625" customWidth="1"/>
-    <col min="5" max="6" width="9.19921875" customWidth="1"/>
-    <col min="7" max="7" width="15.8984375" customWidth="1"/>
-    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="4" max="4" width="13.69921875" customWidth="1"/>
+    <col min="5" max="5" width="10.69921875" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" customWidth="1"/>
+    <col min="7" max="7" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.19921875" customWidth="1"/>
+    <col min="9" max="9" width="15.8984375" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -1280,678 +1397,1263 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="b">
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="b">
+      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="b">
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="b">
+      <c r="C5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" t="b">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
         <v>118</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>104</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>106</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>107</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="b">
+      <c r="C9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" t="b">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
         <v>118</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>109</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>106</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>110</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="b">
+      <c r="C10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" t="b">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
         <v>118</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>111</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>9</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>106</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>112</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>61</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>62</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>63</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="b">
+      <c r="C13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" t="b">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
         <v>118</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>113</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>12</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>106</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>114</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="b">
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" t="b">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
         <v>118</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>113</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
         <v>13</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>106</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>114</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="b">
+      <c r="C15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" t="b">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
         <v>118</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>113</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>14</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>106</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>114</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>66</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="C17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>68</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>69</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>70</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>71</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>72</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="C22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>73</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
-      <c r="C23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>76</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>153</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="C28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>153</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>78</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>80</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>79</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="C31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>81</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
       </c>
-      <c r="C32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>82</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="C33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>83</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="C34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>84</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="C35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>153</v>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>85</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
       </c>
-      <c r="C36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>86</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>87</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
-      <c r="C38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>88</v>
       </c>
       <c r="B39" t="s">
         <v>49</v>
       </c>
-      <c r="C39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>89</v>
       </c>
       <c r="B40" t="s">
         <v>37</v>
       </c>
-      <c r="C40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>90</v>
       </c>
       <c r="B41" t="s">
         <v>38</v>
       </c>
-      <c r="C41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>91</v>
       </c>
       <c r="B42" t="s">
         <v>39</v>
       </c>
-      <c r="C42" t="b">
+      <c r="C42" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>92</v>
       </c>
       <c r="B43" t="s">
         <v>40</v>
       </c>
-      <c r="C43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>93</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
       </c>
-      <c r="C44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>94</v>
       </c>
       <c r="B45" t="s">
         <v>42</v>
       </c>
-      <c r="C45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>95</v>
       </c>
       <c r="B46" t="s">
         <v>43</v>
       </c>
-      <c r="C46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>96</v>
       </c>
       <c r="B47" t="s">
         <v>44</v>
       </c>
-      <c r="C47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>97</v>
       </c>
       <c r="B48" t="s">
         <v>45</v>
       </c>
-      <c r="C48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>98</v>
       </c>
       <c r="B49" t="s">
         <v>46</v>
       </c>
-      <c r="C49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>153</v>
+      </c>
+      <c r="D49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>99</v>
       </c>
       <c r="B50" t="s">
         <v>47</v>
       </c>
-      <c r="C50" t="b">
-        <v>0</v>
+      <c r="C50" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>127</v>
+      </c>
+      <c r="B53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" t="s">
+        <v>124</v>
+      </c>
+      <c r="D53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" t="s">
+        <v>124</v>
+      </c>
+      <c r="D54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>131</v>
+      </c>
+      <c r="B55" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" t="s">
+        <v>124</v>
+      </c>
+      <c r="D56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>137</v>
+      </c>
+      <c r="B58" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" t="s">
+        <v>139</v>
+      </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" t="s">
+        <v>154</v>
+      </c>
+      <c r="J61" t="s">
+        <v>143</v>
+      </c>
+      <c r="K61" t="s">
+        <v>106</v>
+      </c>
+      <c r="L61" t="s">
+        <v>157</v>
+      </c>
+      <c r="M61" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" t="s">
+        <v>139</v>
+      </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" t="s">
+        <v>155</v>
+      </c>
+      <c r="J62" t="s">
+        <v>145</v>
+      </c>
+      <c r="K62" t="s">
+        <v>106</v>
+      </c>
+      <c r="L62" t="s">
+        <v>156</v>
+      </c>
+      <c r="M62" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>146</v>
+      </c>
+      <c r="B63" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" t="s">
+        <v>139</v>
+      </c>
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>148</v>
+      </c>
+      <c r="B64" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>150</v>
+      </c>
+      <c r="B65" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" t="s">
+        <v>139</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working checkpoint (added pid_view_02)
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="293" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96B31127-B83B-424F-B83B-2F35CDFA4653}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EC284E5-05B7-4BEE-9169-5154FCA952F2}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="184">
   <si>
     <t>db_name</t>
   </si>
@@ -516,6 +516,75 @@
   </si>
   <si>
     <t>communication_data_view</t>
+  </si>
+  <si>
+    <t>action_item_status</t>
+  </si>
+  <si>
+    <t>action_value</t>
+  </si>
+  <si>
+    <t>isa_value</t>
+  </si>
+  <si>
+    <t>isa_report_value</t>
+  </si>
+  <si>
+    <t>intent_letter_value</t>
+  </si>
+  <si>
+    <t>ps_agree_value</t>
+  </si>
+  <si>
+    <t>easement_value</t>
+  </si>
+  <si>
+    <t>env_investigation_value</t>
+  </si>
+  <si>
+    <t>title_certificate_value</t>
+  </si>
+  <si>
+    <t>appraisal_value</t>
+  </si>
+  <si>
+    <t>survey_value</t>
+  </si>
+  <si>
+    <t>boundary_agreement_value</t>
+  </si>
+  <si>
+    <t>legal_title_mig_value</t>
+  </si>
+  <si>
+    <t>ecogifts_value</t>
+  </si>
+  <si>
+    <t>approval_cc_value</t>
+  </si>
+  <si>
+    <t>approval_board_value</t>
+  </si>
+  <si>
+    <t>af_phase_01_value</t>
+  </si>
+  <si>
+    <t>af_phase_02_value</t>
+  </si>
+  <si>
+    <t>af_phase_03_value</t>
+  </si>
+  <si>
+    <t>af_ease_transfer_value</t>
+  </si>
+  <si>
+    <t>af_remoteness_letter_value</t>
+  </si>
+  <si>
+    <t>af_field_verified_value</t>
+  </si>
+  <si>
+    <t>llt_funding_value</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1104,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1367,20 +1443,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="4" width="13.69921875" customWidth="1"/>
-    <col min="5" max="5" width="10.69921875" customWidth="1"/>
-    <col min="6" max="6" width="9.19921875" customWidth="1"/>
-    <col min="7" max="7" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.296875" customWidth="1"/>
+    <col min="7" max="7" width="23.09765625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.19921875" customWidth="1"/>
     <col min="9" max="9" width="15.8984375" customWidth="1"/>
     <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
@@ -1440,7 +1515,10 @@
       <c r="C2" t="s">
         <v>153</v>
       </c>
-      <c r="D2" t="b">
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G2" t="b">
@@ -1460,6 +1538,9 @@
       <c r="D3" t="b">
         <v>1</v>
       </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
       <c r="G3" t="b">
         <v>0</v>
       </c>
@@ -1477,6 +1558,9 @@
       <c r="D4" t="b">
         <v>1</v>
       </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
       <c r="G4" t="b">
         <v>0</v>
       </c>
@@ -1494,6 +1578,9 @@
       <c r="D5" t="b">
         <v>1</v>
       </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
@@ -1529,6 +1616,9 @@
       <c r="D6" t="b">
         <v>0</v>
       </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
       <c r="G6" t="b">
         <v>0</v>
       </c>
@@ -1546,6 +1636,9 @@
       <c r="D7" t="b">
         <v>0</v>
       </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
       <c r="G7" t="b">
         <v>0</v>
       </c>
@@ -1563,6 +1656,9 @@
       <c r="D8" t="b">
         <v>0</v>
       </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
       <c r="G8" t="b">
         <v>0</v>
       </c>
@@ -1580,6 +1676,9 @@
       <c r="D9" t="b">
         <v>1</v>
       </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
       <c r="G9" t="b">
         <v>0</v>
       </c>
@@ -1615,6 +1714,9 @@
       <c r="D10" t="b">
         <v>1</v>
       </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
       <c r="G10" t="b">
         <v>0</v>
       </c>
@@ -1650,6 +1752,9 @@
       <c r="D11" t="b">
         <v>0</v>
       </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
       <c r="G11" t="b">
         <v>0</v>
       </c>
@@ -1667,6 +1772,9 @@
       <c r="D12" t="b">
         <v>0</v>
       </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
       <c r="G12" t="b">
         <v>0</v>
       </c>
@@ -1684,6 +1792,9 @@
       <c r="D13" t="b">
         <v>1</v>
       </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
       <c r="G13" t="b">
         <v>0</v>
       </c>
@@ -1719,6 +1830,9 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
       <c r="G14" t="b">
         <v>0</v>
       </c>
@@ -1754,6 +1868,9 @@
       <c r="D15" t="b">
         <v>1</v>
       </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
       <c r="G15" t="b">
         <v>0</v>
       </c>
@@ -1789,11 +1906,32 @@
       <c r="D16" t="b">
         <v>0</v>
       </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
       <c r="G16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" t="s">
+        <v>161</v>
+      </c>
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16" t="s">
+        <v>162</v>
+      </c>
+      <c r="M16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -1806,11 +1944,32 @@
       <c r="D17" t="b">
         <v>0</v>
       </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
       <c r="G17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>118</v>
+      </c>
+      <c r="I17" t="s">
+        <v>161</v>
+      </c>
+      <c r="J17" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" t="s">
+        <v>106</v>
+      </c>
+      <c r="L17" t="s">
+        <v>162</v>
+      </c>
+      <c r="M17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1823,11 +1982,32 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
       <c r="G18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" t="s">
+        <v>161</v>
+      </c>
+      <c r="J18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" t="s">
+        <v>106</v>
+      </c>
+      <c r="L18" t="s">
+        <v>162</v>
+      </c>
+      <c r="M18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -1840,11 +2020,32 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
       <c r="G19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" t="s">
+        <v>161</v>
+      </c>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19" t="s">
+        <v>162</v>
+      </c>
+      <c r="M19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1857,11 +2058,32 @@
       <c r="D20" t="b">
         <v>0</v>
       </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
       <c r="G20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" t="s">
+        <v>161</v>
+      </c>
+      <c r="J20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" t="s">
+        <v>106</v>
+      </c>
+      <c r="L20" t="s">
+        <v>162</v>
+      </c>
+      <c r="M20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -1874,11 +2096,32 @@
       <c r="D21" t="b">
         <v>0</v>
       </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
       <c r="G21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>118</v>
+      </c>
+      <c r="I21" t="s">
+        <v>161</v>
+      </c>
+      <c r="J21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" t="s">
+        <v>106</v>
+      </c>
+      <c r="L21" t="s">
+        <v>162</v>
+      </c>
+      <c r="M21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -1891,11 +2134,32 @@
       <c r="D22" t="b">
         <v>0</v>
       </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
       <c r="G22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>118</v>
+      </c>
+      <c r="I22" t="s">
+        <v>161</v>
+      </c>
+      <c r="J22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" t="s">
+        <v>106</v>
+      </c>
+      <c r="L22" t="s">
+        <v>162</v>
+      </c>
+      <c r="M22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1908,11 +2172,32 @@
       <c r="D23" t="b">
         <v>0</v>
       </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
       <c r="G23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23" t="s">
+        <v>161</v>
+      </c>
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" t="s">
+        <v>106</v>
+      </c>
+      <c r="L23" t="s">
+        <v>162</v>
+      </c>
+      <c r="M23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1925,11 +2210,14 @@
       <c r="D24" t="b">
         <v>0</v>
       </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
       <c r="G24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -1942,11 +2230,14 @@
       <c r="D25" t="b">
         <v>0</v>
       </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1959,11 +2250,32 @@
       <c r="D26" t="b">
         <v>0</v>
       </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
       <c r="G26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>118</v>
+      </c>
+      <c r="I26" t="s">
+        <v>161</v>
+      </c>
+      <c r="J26" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" t="s">
+        <v>106</v>
+      </c>
+      <c r="L26" t="s">
+        <v>162</v>
+      </c>
+      <c r="M26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -1976,11 +2288,32 @@
       <c r="D27" t="b">
         <v>0</v>
       </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
       <c r="G27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>118</v>
+      </c>
+      <c r="I27" t="s">
+        <v>161</v>
+      </c>
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" t="s">
+        <v>106</v>
+      </c>
+      <c r="L27" t="s">
+        <v>162</v>
+      </c>
+      <c r="M27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -1993,11 +2326,32 @@
       <c r="D28" t="b">
         <v>0</v>
       </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
       <c r="G28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" t="s">
+        <v>161</v>
+      </c>
+      <c r="J28" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" t="s">
+        <v>106</v>
+      </c>
+      <c r="L28" t="s">
+        <v>162</v>
+      </c>
+      <c r="M28" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -2010,11 +2364,32 @@
       <c r="D29" t="b">
         <v>0</v>
       </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
       <c r="G29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>118</v>
+      </c>
+      <c r="I29" t="s">
+        <v>161</v>
+      </c>
+      <c r="J29" t="s">
+        <v>27</v>
+      </c>
+      <c r="K29" t="s">
+        <v>106</v>
+      </c>
+      <c r="L29" t="s">
+        <v>162</v>
+      </c>
+      <c r="M29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -2027,11 +2402,32 @@
       <c r="D30" t="b">
         <v>0</v>
       </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
       <c r="G30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" t="s">
+        <v>161</v>
+      </c>
+      <c r="J30" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" t="s">
+        <v>106</v>
+      </c>
+      <c r="L30" t="s">
+        <v>162</v>
+      </c>
+      <c r="M30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -2044,11 +2440,32 @@
       <c r="D31" t="b">
         <v>0</v>
       </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
       <c r="G31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>118</v>
+      </c>
+      <c r="I31" t="s">
+        <v>161</v>
+      </c>
+      <c r="J31" t="s">
+        <v>29</v>
+      </c>
+      <c r="K31" t="s">
+        <v>106</v>
+      </c>
+      <c r="L31" t="s">
+        <v>162</v>
+      </c>
+      <c r="M31" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -2061,11 +2478,14 @@
       <c r="D32" t="b">
         <v>0</v>
       </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
       <c r="G32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -2078,11 +2498,32 @@
       <c r="D33" t="b">
         <v>0</v>
       </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
       <c r="G33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33" t="s">
+        <v>161</v>
+      </c>
+      <c r="J33" t="s">
+        <v>31</v>
+      </c>
+      <c r="K33" t="s">
+        <v>106</v>
+      </c>
+      <c r="L33" t="s">
+        <v>162</v>
+      </c>
+      <c r="M33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -2095,11 +2536,32 @@
       <c r="D34" t="b">
         <v>0</v>
       </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
       <c r="G34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>118</v>
+      </c>
+      <c r="I34" t="s">
+        <v>161</v>
+      </c>
+      <c r="J34" t="s">
+        <v>32</v>
+      </c>
+      <c r="K34" t="s">
+        <v>106</v>
+      </c>
+      <c r="L34" t="s">
+        <v>162</v>
+      </c>
+      <c r="M34" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -2112,11 +2574,32 @@
       <c r="D35" t="b">
         <v>0</v>
       </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
       <c r="G35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>118</v>
+      </c>
+      <c r="I35" t="s">
+        <v>161</v>
+      </c>
+      <c r="J35" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" t="s">
+        <v>106</v>
+      </c>
+      <c r="L35" t="s">
+        <v>162</v>
+      </c>
+      <c r="M35" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -2129,11 +2612,32 @@
       <c r="D36" t="b">
         <v>0</v>
       </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
       <c r="G36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>118</v>
+      </c>
+      <c r="I36" t="s">
+        <v>161</v>
+      </c>
+      <c r="J36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K36" t="s">
+        <v>106</v>
+      </c>
+      <c r="L36" t="s">
+        <v>162</v>
+      </c>
+      <c r="M36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2146,11 +2650,32 @@
       <c r="D37" t="b">
         <v>0</v>
       </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
       <c r="G37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>118</v>
+      </c>
+      <c r="I37" t="s">
+        <v>161</v>
+      </c>
+      <c r="J37" t="s">
+        <v>35</v>
+      </c>
+      <c r="K37" t="s">
+        <v>106</v>
+      </c>
+      <c r="L37" t="s">
+        <v>162</v>
+      </c>
+      <c r="M37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -2163,11 +2688,32 @@
       <c r="D38" t="b">
         <v>0</v>
       </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
       <c r="G38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>118</v>
+      </c>
+      <c r="I38" t="s">
+        <v>161</v>
+      </c>
+      <c r="J38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K38" t="s">
+        <v>106</v>
+      </c>
+      <c r="L38" t="s">
+        <v>162</v>
+      </c>
+      <c r="M38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2180,11 +2726,32 @@
       <c r="D39" t="b">
         <v>0</v>
       </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
       <c r="G39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>118</v>
+      </c>
+      <c r="I39" t="s">
+        <v>161</v>
+      </c>
+      <c r="J39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K39" t="s">
+        <v>106</v>
+      </c>
+      <c r="L39" t="s">
+        <v>162</v>
+      </c>
+      <c r="M39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>89</v>
       </c>
@@ -2197,11 +2764,20 @@
       <c r="D40" t="b">
         <v>0</v>
       </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
       <c r="G40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>118</v>
+      </c>
+      <c r="K40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -2214,11 +2790,20 @@
       <c r="D41" t="b">
         <v>0</v>
       </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
       <c r="G41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>118</v>
+      </c>
+      <c r="K41" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -2231,11 +2816,20 @@
       <c r="D42" t="b">
         <v>1</v>
       </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
       <c r="G42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>118</v>
+      </c>
+      <c r="K42" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -2248,11 +2842,20 @@
       <c r="D43" t="b">
         <v>0</v>
       </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
       <c r="G43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" t="s">
+        <v>118</v>
+      </c>
+      <c r="K43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -2265,11 +2868,20 @@
       <c r="D44" t="b">
         <v>0</v>
       </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
       <c r="G44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" t="s">
+        <v>118</v>
+      </c>
+      <c r="K44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -2282,11 +2894,20 @@
       <c r="D45" t="b">
         <v>0</v>
       </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
       <c r="G45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45" t="s">
+        <v>118</v>
+      </c>
+      <c r="K45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -2299,11 +2920,20 @@
       <c r="D46" t="b">
         <v>0</v>
       </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
       <c r="G46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>118</v>
+      </c>
+      <c r="K46" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -2316,11 +2946,20 @@
       <c r="D47" t="b">
         <v>0</v>
       </c>
+      <c r="E47" t="b">
+        <v>0</v>
+      </c>
       <c r="G47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47" t="s">
+        <v>118</v>
+      </c>
+      <c r="K47" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -2333,8 +2972,17 @@
       <c r="D48" t="b">
         <v>0</v>
       </c>
+      <c r="E48" t="b">
+        <v>0</v>
+      </c>
       <c r="G48" t="b">
         <v>0</v>
+      </c>
+      <c r="H48" t="s">
+        <v>118</v>
+      </c>
+      <c r="K48" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
@@ -2350,8 +2998,17 @@
       <c r="D49" t="b">
         <v>0</v>
       </c>
+      <c r="E49" t="b">
+        <v>0</v>
+      </c>
       <c r="G49" t="b">
         <v>0</v>
+      </c>
+      <c r="H49" t="s">
+        <v>118</v>
+      </c>
+      <c r="K49" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
@@ -2367,8 +3024,17 @@
       <c r="D50" t="b">
         <v>0</v>
       </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
       <c r="G50" t="b">
         <v>0</v>
+      </c>
+      <c r="H50" t="s">
+        <v>118</v>
+      </c>
+      <c r="K50" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
@@ -2384,8 +3050,17 @@
       <c r="D51" t="b">
         <v>0</v>
       </c>
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
       <c r="G51" t="b">
         <v>0</v>
+      </c>
+      <c r="H51" t="s">
+        <v>118</v>
+      </c>
+      <c r="K51" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
@@ -2401,8 +3076,17 @@
       <c r="D52" t="b">
         <v>0</v>
       </c>
+      <c r="E52" t="b">
+        <v>0</v>
+      </c>
       <c r="G52" t="b">
         <v>0</v>
+      </c>
+      <c r="H52" t="s">
+        <v>118</v>
+      </c>
+      <c r="K52" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
@@ -2418,8 +3102,17 @@
       <c r="D53" t="b">
         <v>0</v>
       </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
       <c r="G53" t="b">
         <v>0</v>
+      </c>
+      <c r="H53" t="s">
+        <v>118</v>
+      </c>
+      <c r="K53" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
@@ -2435,8 +3128,17 @@
       <c r="D54" t="b">
         <v>0</v>
       </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
       <c r="G54" t="b">
         <v>0</v>
+      </c>
+      <c r="H54" t="s">
+        <v>118</v>
+      </c>
+      <c r="K54" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
@@ -2452,8 +3154,17 @@
       <c r="D55" t="b">
         <v>0</v>
       </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
       <c r="G55" t="b">
         <v>0</v>
+      </c>
+      <c r="H55" t="s">
+        <v>118</v>
+      </c>
+      <c r="K55" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
@@ -2469,8 +3180,17 @@
       <c r="D56" t="b">
         <v>0</v>
       </c>
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
       <c r="G56" t="b">
         <v>0</v>
+      </c>
+      <c r="H56" t="s">
+        <v>118</v>
+      </c>
+      <c r="K56" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
@@ -2486,8 +3206,17 @@
       <c r="D57" t="b">
         <v>0</v>
       </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
       <c r="G57" t="b">
         <v>0</v>
+      </c>
+      <c r="H57" t="s">
+        <v>118</v>
+      </c>
+      <c r="K57" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
@@ -2503,8 +3232,17 @@
       <c r="D58" t="b">
         <v>0</v>
       </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
       <c r="G58" t="b">
         <v>0</v>
+      </c>
+      <c r="H58" t="s">
+        <v>118</v>
+      </c>
+      <c r="K58" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
@@ -2520,8 +3258,17 @@
       <c r="D59" t="b">
         <v>0</v>
       </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
       <c r="G59" t="b">
         <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>118</v>
+      </c>
+      <c r="K59" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
@@ -2537,8 +3284,17 @@
       <c r="D60" t="b">
         <v>0</v>
       </c>
+      <c r="E60" t="b">
+        <v>0</v>
+      </c>
       <c r="G60" t="b">
         <v>1</v>
+      </c>
+      <c r="H60" t="s">
+        <v>118</v>
+      </c>
+      <c r="K60" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
@@ -2554,8 +3310,14 @@
       <c r="D61" t="b">
         <v>0</v>
       </c>
+      <c r="E61" t="b">
+        <v>0</v>
+      </c>
       <c r="G61" t="b">
         <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>118</v>
       </c>
       <c r="I61" t="s">
         <v>154</v>
@@ -2586,8 +3348,14 @@
       <c r="D62" t="b">
         <v>0</v>
       </c>
+      <c r="E62" t="b">
+        <v>0</v>
+      </c>
       <c r="G62" t="b">
         <v>1</v>
+      </c>
+      <c r="H62" t="s">
+        <v>118</v>
       </c>
       <c r="I62" t="s">
         <v>155</v>
@@ -2618,8 +3386,14 @@
       <c r="D63" t="b">
         <v>0</v>
       </c>
+      <c r="E63" t="b">
+        <v>0</v>
+      </c>
       <c r="G63" t="b">
         <v>1</v>
+      </c>
+      <c r="H63" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
@@ -2635,11 +3409,17 @@
       <c r="D64" t="b">
         <v>0</v>
       </c>
+      <c r="E64" t="b">
+        <v>0</v>
+      </c>
       <c r="G64" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H64" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>150</v>
       </c>
@@ -2652,12 +3432,24 @@
       <c r="D65" t="b">
         <v>0</v>
       </c>
+      <c r="E65" t="b">
+        <v>0</v>
+      </c>
       <c r="G65" t="b">
         <v>1</v>
+      </c>
+      <c r="H65" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="D1:G65">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor action item tracking module for improved UI and functionality 🎨✨
- Updated UI components to enhance user experience, including:
  - Changed card to not be full screen for better layout.
  - Added a new button to refresh the data viewer.
  - Renamed input fields for clarity (e.g., "checklist_fields" to "action_item_fields").
  - Adjusted column widths for a more balanced layout.

- Improved server logic with input validation to ensure required fields are filled before submission.
- Added functionality to refresh the database and clear inputs effectively.
- Updated data viewer integration to streamline data presentation.

Untracked files added:
- Updated the `df_views.xlsx` file to reflect changes in action item fields and values.
- Enhanced Docker notes for clearer instructions on updating app files within the container.
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="399" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F03B81F-436C-4FD8-82B3-46182B9719BD}"/>
+  <xr:revisionPtr revIDLastSave="411" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37ED3A2C-4756-4B37-BC1D-F074C922F984}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="names" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">names!$A$1:$N$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">names!$A$1:$O$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="190">
   <si>
     <t>db_name</t>
   </si>
@@ -603,6 +603,9 @@
   </si>
   <si>
     <t>pid_view_03</t>
+  </si>
+  <si>
+    <t>action_item_fields</t>
   </si>
 </sst>
 </file>
@@ -1459,32 +1462,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" customWidth="1"/>
     <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="13.296875" customWidth="1"/>
-    <col min="8" max="8" width="23.09765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.19921875" customWidth="1"/>
-    <col min="10" max="10" width="15.8984375" customWidth="1"/>
-    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.296875" customWidth="1"/>
+    <col min="9" max="9" width="23.09765625" customWidth="1"/>
+    <col min="10" max="10" width="9.19921875" customWidth="1"/>
+    <col min="11" max="11" width="15.8984375" customWidth="1"/>
+    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -1510,25 +1513,28 @@
         <v>159</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1553,8 +1559,11 @@
       <c r="H2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1579,8 +1588,11 @@
       <c r="H3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1605,8 +1617,11 @@
       <c r="H4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1631,26 +1646,29 @@
       <c r="H5" t="b">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
         <v>118</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>104</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>4</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>106</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>107</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1675,8 +1693,11 @@
       <c r="H6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1701,8 +1722,11 @@
       <c r="H7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1727,8 +1751,11 @@
       <c r="H8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1753,26 +1780,29 @@
       <c r="H9" t="b">
         <v>0</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
         <v>118</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>109</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>8</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>106</v>
-      </c>
-      <c r="M9" t="s">
-        <v>110</v>
       </c>
       <c r="N9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="O9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -1797,26 +1827,29 @@
       <c r="H10" t="b">
         <v>0</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
         <v>118</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>111</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>9</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>106</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>112</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1841,8 +1874,11 @@
       <c r="H11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -1867,8 +1903,11 @@
       <c r="H12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -1893,26 +1932,29 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
         <v>118</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>113</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>12</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>106</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>114</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1937,26 +1979,29 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
         <v>118</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>113</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>13</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>106</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>114</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1981,26 +2026,29 @@
       <c r="H15" t="b">
         <v>0</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
         <v>118</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>113</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>14</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>106</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>114</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -2025,26 +2073,29 @@
       <c r="H16" t="b">
         <v>0</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
         <v>118</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>160</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>15</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>106</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>161</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -2069,26 +2120,29 @@
       <c r="H17" t="b">
         <v>0</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
         <v>118</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>160</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>48</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>106</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>161</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -2113,26 +2167,29 @@
       <c r="H18" t="b">
         <v>0</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
         <v>118</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>160</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>16</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>106</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>161</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -2157,26 +2214,29 @@
       <c r="H19" t="b">
         <v>0</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
         <v>118</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>160</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>17</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>106</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>161</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -2201,26 +2261,29 @@
       <c r="H20" t="b">
         <v>0</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
         <v>118</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>160</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>18</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>106</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>161</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -2245,26 +2308,29 @@
       <c r="H21" t="b">
         <v>0</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
         <v>118</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>160</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>19</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>106</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>161</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2289,26 +2355,29 @@
       <c r="H22" t="b">
         <v>0</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
         <v>118</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>160</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>20</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>106</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>161</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -2333,26 +2402,29 @@
       <c r="H23" t="b">
         <v>0</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
         <v>118</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>160</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>21</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>106</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>161</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -2377,8 +2449,11 @@
       <c r="H24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2403,8 +2478,11 @@
       <c r="H25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -2429,26 +2507,29 @@
       <c r="H26" t="b">
         <v>0</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
         <v>118</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>160</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>24</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>106</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>161</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -2473,26 +2554,29 @@
       <c r="H27" t="b">
         <v>0</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
         <v>118</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>160</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>25</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>106</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>161</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -2517,26 +2601,29 @@
       <c r="H28" t="b">
         <v>0</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
         <v>118</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>160</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>26</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>106</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>161</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -2561,26 +2648,29 @@
       <c r="H29" t="b">
         <v>0</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
         <v>118</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>160</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>27</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>106</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>161</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>80</v>
       </c>
@@ -2605,26 +2695,29 @@
       <c r="H30" t="b">
         <v>0</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
         <v>118</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>160</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>28</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>106</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>161</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -2649,26 +2742,29 @@
       <c r="H31" t="b">
         <v>0</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
         <v>118</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>160</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>29</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>106</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>161</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -2693,8 +2789,11 @@
       <c r="H32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -2719,26 +2818,29 @@
       <c r="H33" t="b">
         <v>0</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
         <v>118</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>160</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>31</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>106</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>161</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -2763,26 +2865,29 @@
       <c r="H34" t="b">
         <v>0</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
         <v>118</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>160</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>32</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>106</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>161</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -2807,26 +2912,29 @@
       <c r="H35" t="b">
         <v>0</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
         <v>118</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>160</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>33</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>106</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>161</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -2851,26 +2959,29 @@
       <c r="H36" t="b">
         <v>0</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
         <v>118</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>160</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>34</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>106</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>161</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2895,26 +3006,29 @@
       <c r="H37" t="b">
         <v>0</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
         <v>118</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>160</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>35</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>106</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>161</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -2939,26 +3053,29 @@
       <c r="H38" t="b">
         <v>0</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
         <v>118</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>160</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>36</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>106</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>161</v>
       </c>
-      <c r="N38" t="s">
+      <c r="O38" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2983,26 +3100,29 @@
       <c r="H39" t="b">
         <v>0</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
         <v>118</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>160</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>49</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>106</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>161</v>
       </c>
-      <c r="N39" t="s">
+      <c r="O39" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>89</v>
       </c>
@@ -3027,8 +3147,11 @@
       <c r="H40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -3053,8 +3176,11 @@
       <c r="H41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -3079,8 +3205,11 @@
       <c r="H42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -3105,8 +3234,11 @@
       <c r="H43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -3131,8 +3263,11 @@
       <c r="H44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -3157,8 +3292,11 @@
       <c r="H45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -3183,8 +3321,11 @@
       <c r="H46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -3209,8 +3350,11 @@
       <c r="H47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -3235,8 +3379,11 @@
       <c r="H48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -3261,8 +3408,11 @@
       <c r="H49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -3287,8 +3437,11 @@
       <c r="H50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>122</v>
       </c>
@@ -3313,8 +3466,11 @@
       <c r="H51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>124</v>
       </c>
@@ -3339,8 +3495,11 @@
       <c r="H52" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>126</v>
       </c>
@@ -3365,8 +3524,11 @@
       <c r="H53" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>128</v>
       </c>
@@ -3391,8 +3553,11 @@
       <c r="H54" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>130</v>
       </c>
@@ -3417,8 +3582,11 @@
       <c r="H55" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>132</v>
       </c>
@@ -3443,8 +3611,11 @@
       <c r="H56" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -3469,8 +3640,11 @@
       <c r="H57" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>147</v>
       </c>
@@ -3495,8 +3669,11 @@
       <c r="H58" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>136</v>
       </c>
@@ -3521,8 +3698,11 @@
       <c r="H59" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>122</v>
       </c>
@@ -3547,8 +3727,11 @@
       <c r="H60" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -3573,8 +3756,11 @@
       <c r="H61" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>141</v>
       </c>
@@ -3599,26 +3785,29 @@
       <c r="H62" t="b">
         <v>1</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62" t="b">
+        <v>0</v>
+      </c>
+      <c r="J62" t="s">
         <v>118</v>
       </c>
-      <c r="J62" t="s">
+      <c r="K62" t="s">
         <v>153</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" t="s">
         <v>142</v>
       </c>
-      <c r="L62" t="s">
+      <c r="M62" t="s">
         <v>106</v>
       </c>
-      <c r="M62" t="s">
+      <c r="N62" t="s">
         <v>156</v>
       </c>
-      <c r="N62" t="s">
+      <c r="O62" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>143</v>
       </c>
@@ -3643,26 +3832,29 @@
       <c r="H63" t="b">
         <v>1</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+      <c r="J63" t="s">
         <v>118</v>
       </c>
-      <c r="J63" t="s">
+      <c r="K63" t="s">
         <v>154</v>
       </c>
-      <c r="K63" t="s">
+      <c r="L63" t="s">
         <v>144</v>
       </c>
-      <c r="L63" t="s">
+      <c r="M63" t="s">
         <v>106</v>
       </c>
-      <c r="M63" t="s">
+      <c r="N63" t="s">
         <v>155</v>
       </c>
-      <c r="N63" t="s">
+      <c r="O63" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -3687,8 +3879,11 @@
       <c r="H64" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -3713,8 +3908,11 @@
       <c r="H65" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -3739,8 +3937,11 @@
       <c r="H66" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>51</v>
       </c>
@@ -3765,26 +3966,29 @@
       <c r="H67" t="b">
         <v>0</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" t="b">
+        <v>0</v>
+      </c>
+      <c r="J67" t="s">
         <v>118</v>
       </c>
-      <c r="J67" t="s">
-        <v>152</v>
-      </c>
       <c r="K67" t="s">
+        <v>152</v>
+      </c>
+      <c r="L67" t="s">
         <v>185</v>
       </c>
-      <c r="L67" t="s">
+      <c r="M67" t="s">
         <v>106</v>
       </c>
-      <c r="M67" t="s">
-        <v>1</v>
-      </c>
       <c r="N67" t="s">
+        <v>1</v>
+      </c>
+      <c r="O67" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>136</v>
       </c>
@@ -3809,8 +4013,11 @@
       <c r="H68" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>141</v>
       </c>
@@ -3835,26 +4042,29 @@
       <c r="H69" t="b">
         <v>0</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I69" t="b">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
         <v>118</v>
       </c>
-      <c r="J69" t="s">
+      <c r="K69" t="s">
         <v>153</v>
       </c>
-      <c r="K69" t="s">
+      <c r="L69" t="s">
         <v>142</v>
       </c>
-      <c r="L69" t="s">
+      <c r="M69" t="s">
         <v>106</v>
       </c>
-      <c r="M69" t="s">
+      <c r="N69" t="s">
         <v>156</v>
       </c>
-      <c r="N69" t="s">
+      <c r="O69" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>143</v>
       </c>
@@ -3879,26 +4089,29 @@
       <c r="H70" t="b">
         <v>0</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
         <v>118</v>
       </c>
-      <c r="J70" t="s">
+      <c r="K70" t="s">
         <v>154</v>
       </c>
-      <c r="K70" t="s">
+      <c r="L70" t="s">
         <v>144</v>
       </c>
-      <c r="L70" t="s">
+      <c r="M70" t="s">
         <v>106</v>
       </c>
-      <c r="M70" t="s">
+      <c r="N70" t="s">
         <v>155</v>
       </c>
-      <c r="N70" t="s">
+      <c r="O70" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>145</v>
       </c>
@@ -3923,8 +4136,11 @@
       <c r="H71" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -3949,8 +4165,11 @@
       <c r="H72" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -3975,17 +4194,14 @@
       <c r="H73" t="b">
         <v>0</v>
       </c>
+      <c r="I73" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N73" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O73" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}"/>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D1:H1 G2:G16 D2:F57 H2:H57 G20:G34 G38:G52 G56:G57 D58:H58 D59:F68 H59:H68 G59:G73">
+  <conditionalFormatting sqref="D1:I1 H2:I2 G2:G16 D2:F57 H3:H57 I3:I73 G20:G34 G38:G52 G56:G57 D58:H58 D59:F68 H59:H68 G59:G73">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add securement action description input and update server logic ✏️📝
- Introduced a new text area input for "Securement action description" in the UI to capture additional notes related to action items.
- Updated the server logic to handle the new input, ensuring that securement action notes are processed correctly.
- Modified the Excel file `df_views.xlsx` to reflect changes in the data structure, which includes updates to the action item fields.
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="411" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37ED3A2C-4756-4B37-BC1D-F074C922F984}"/>
+  <xr:revisionPtr revIDLastSave="450" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC35E329-B45F-4E52-908C-B8EAC05D5359}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
+    <workbookView xWindow="-192" yWindow="-192" windowWidth="23424" windowHeight="12624" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">names!$A$1:$O$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">names!$A$1:$O$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="192">
   <si>
     <t>db_name</t>
   </si>
@@ -53,12 +53,6 @@
     <t>property_id</t>
   </si>
   <si>
-    <t>size_acre</t>
-  </si>
-  <si>
-    <t>size_ha</t>
-  </si>
-  <si>
     <t>core_property</t>
   </si>
   <si>
@@ -209,12 +203,6 @@
     <t>Property Name</t>
   </si>
   <si>
-    <t>Size (acres)</t>
-  </si>
-  <si>
-    <t>Size (ha)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Phase </t>
   </si>
   <si>
@@ -606,6 +594,24 @@
   </si>
   <si>
     <t>action_item_fields</t>
+  </si>
+  <si>
+    <t>Phase Description</t>
+  </si>
+  <si>
+    <t>phase_id_description</t>
+  </si>
+  <si>
+    <t>securement_action_notes</t>
+  </si>
+  <si>
+    <t>Securement Action Notes</t>
+  </si>
+  <si>
+    <t>size_acres_confirmed</t>
+  </si>
+  <si>
+    <t>Size (acres) Confirmed</t>
   </si>
 </sst>
 </file>
@@ -1462,23 +1468,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" customWidth="1"/>
-    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="13.296875" customWidth="1"/>
-    <col min="8" max="8" width="8.296875" customWidth="1"/>
-    <col min="9" max="9" width="23.09765625" customWidth="1"/>
+    <col min="3" max="3" width="20.796875" customWidth="1"/>
+    <col min="4" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.59765625" customWidth="1"/>
+    <col min="9" max="9" width="18.09765625" customWidth="1"/>
     <col min="10" max="10" width="9.19921875" customWidth="1"/>
     <col min="11" max="11" width="15.8984375" customWidth="1"/>
     <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
@@ -1489,60 +1494,60 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D2" s="1" t="b">
         <v>1</v>
@@ -1565,13 +1570,13 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1594,13 +1599,13 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1623,13 +1628,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -1650,33 +1655,33 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L5" t="s">
         <v>4</v>
       </c>
       <c r="M5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="O5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1699,22 +1704,22 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
       <c r="F7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -1724,26 +1729,44 @@
       </c>
       <c r="I7" t="b">
         <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>114</v>
+      </c>
+      <c r="K7" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>102</v>
+      </c>
+      <c r="N7" t="s">
+        <v>106</v>
+      </c>
+      <c r="O7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>186</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -1757,13 +1780,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -1784,42 +1807,42 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -1829,35 +1852,17 @@
       </c>
       <c r="I10" t="b">
         <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>118</v>
-      </c>
-      <c r="K10" t="s">
-        <v>111</v>
-      </c>
-      <c r="L10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10" t="s">
-        <v>106</v>
-      </c>
-      <c r="N10" t="s">
-        <v>112</v>
-      </c>
-      <c r="O10" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1880,22 +1885,22 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -1905,17 +1910,35 @@
       </c>
       <c r="I12" t="b">
         <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>114</v>
+      </c>
+      <c r="K12" t="s">
+        <v>109</v>
+      </c>
+      <c r="L12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" t="s">
+        <v>102</v>
+      </c>
+      <c r="N12" t="s">
+        <v>110</v>
+      </c>
+      <c r="O12" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1936,33 +1959,33 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="O13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -1983,42 +2006,42 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K14" t="s">
+        <v>109</v>
+      </c>
+      <c r="L14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" t="s">
+        <v>102</v>
+      </c>
+      <c r="N14" t="s">
+        <v>110</v>
+      </c>
+      <c r="O14" t="s">
         <v>113</v>
-      </c>
-      <c r="L14" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" t="s">
-        <v>106</v>
-      </c>
-      <c r="N14" t="s">
-        <v>114</v>
-      </c>
-      <c r="O14" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -2027,36 +2050,36 @@
         <v>0</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K15" t="s">
-        <v>113</v>
+        <v>156</v>
       </c>
       <c r="L15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N15" t="s">
-        <v>114</v>
+        <v>157</v>
       </c>
       <c r="O15" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -2077,33 +2100,33 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L16" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="M16" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -2124,33 +2147,33 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K17" t="s">
+        <v>156</v>
+      </c>
+      <c r="L17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" t="s">
+        <v>102</v>
+      </c>
+      <c r="N17" t="s">
+        <v>157</v>
+      </c>
+      <c r="O17" t="s">
         <v>160</v>
-      </c>
-      <c r="L17" t="s">
-        <v>48</v>
-      </c>
-      <c r="M17" t="s">
-        <v>106</v>
-      </c>
-      <c r="N17" t="s">
-        <v>161</v>
-      </c>
-      <c r="O17" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -2171,33 +2194,33 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N18" t="s">
+        <v>157</v>
+      </c>
+      <c r="O18" t="s">
         <v>161</v>
-      </c>
-      <c r="O18" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -2218,33 +2241,33 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K19" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N19" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O19" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -2265,33 +2288,33 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K20" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -2312,33 +2335,33 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K21" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M21" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N21" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O21" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -2359,39 +2382,39 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K22" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M22" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N22" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
       </c>
       <c r="E23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -2403,36 +2426,18 @@
         <v>0</v>
       </c>
       <c r="I23" t="b">
-        <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>118</v>
-      </c>
-      <c r="K23" t="s">
-        <v>160</v>
-      </c>
-      <c r="L23" t="s">
-        <v>21</v>
-      </c>
-      <c r="M23" t="s">
-        <v>106</v>
-      </c>
-      <c r="N23" t="s">
-        <v>161</v>
-      </c>
-      <c r="O23" t="s">
-        <v>169</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -2455,19 +2460,19 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
       </c>
       <c r="E25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -2479,18 +2484,36 @@
         <v>0</v>
       </c>
       <c r="I25" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" t="s">
+        <v>156</v>
+      </c>
+      <c r="L25" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" t="s">
+        <v>102</v>
+      </c>
+      <c r="N25" t="s">
+        <v>157</v>
+      </c>
+      <c r="O25" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -2511,33 +2534,33 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K26" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M26" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N26" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -2558,33 +2581,33 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K27" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N27" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O27" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -2605,33 +2628,33 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K28" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M28" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N28" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O28" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -2652,33 +2675,33 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K29" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M29" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N29" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O29" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -2699,39 +2722,39 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K30" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M30" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N30" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O30" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
       </c>
       <c r="E31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -2743,42 +2766,24 @@
         <v>0</v>
       </c>
       <c r="I31" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" t="s">
-        <v>118</v>
-      </c>
-      <c r="K31" t="s">
-        <v>160</v>
-      </c>
-      <c r="L31" t="s">
-        <v>29</v>
-      </c>
-      <c r="M31" t="s">
-        <v>106</v>
-      </c>
-      <c r="N31" t="s">
-        <v>161</v>
-      </c>
-      <c r="O31" t="s">
-        <v>175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
       </c>
       <c r="E32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -2790,18 +2795,36 @@
         <v>0</v>
       </c>
       <c r="I32" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>114</v>
+      </c>
+      <c r="K32" t="s">
+        <v>156</v>
+      </c>
+      <c r="L32" t="s">
+        <v>29</v>
+      </c>
+      <c r="M32" t="s">
+        <v>102</v>
+      </c>
+      <c r="N32" t="s">
+        <v>157</v>
+      </c>
+      <c r="O32" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -2822,33 +2845,33 @@
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K33" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O33" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -2869,33 +2892,33 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K34" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M34" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N34" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O34" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -2916,33 +2939,33 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K35" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N35" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O35" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -2963,33 +2986,33 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K36" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O36" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -3010,33 +3033,33 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K37" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M37" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N37" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -3054,36 +3077,36 @@
         <v>0</v>
       </c>
       <c r="I38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K38" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L38" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="M38" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N38" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="O38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>189</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>188</v>
       </c>
       <c r="C39" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -3102,35 +3125,17 @@
       </c>
       <c r="I39" t="b">
         <v>0</v>
-      </c>
-      <c r="J39" t="s">
-        <v>118</v>
-      </c>
-      <c r="K39" t="s">
-        <v>160</v>
-      </c>
-      <c r="L39" t="s">
-        <v>49</v>
-      </c>
-      <c r="M39" t="s">
-        <v>106</v>
-      </c>
-      <c r="N39" t="s">
-        <v>161</v>
-      </c>
-      <c r="O39" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -3153,13 +3158,13 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -3182,13 +3187,13 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -3211,13 +3216,13 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -3240,13 +3245,13 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -3269,13 +3274,13 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -3298,13 +3303,13 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -3327,13 +3332,13 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -3356,13 +3361,13 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -3385,13 +3390,13 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -3414,13 +3419,13 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -3443,13 +3448,13 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -3472,13 +3477,13 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="B52" t="s">
-        <v>125</v>
+        <v>190</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -3501,13 +3506,13 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="C53" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -3530,13 +3535,13 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B54" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -3559,13 +3564,13 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -3588,13 +3593,13 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B56" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -3617,13 +3622,13 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C57" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -3646,13 +3651,13 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="B58" t="s">
-        <v>187</v>
+        <v>129</v>
       </c>
       <c r="C58" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -3675,13 +3680,13 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C59" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -3704,13 +3709,13 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>183</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -3725,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="H60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="b">
         <v>0</v>
@@ -3733,13 +3738,13 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C61" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -3754,7 +3759,7 @@
         <v>0</v>
       </c>
       <c r="H61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="b">
         <v>0</v>
@@ -3762,13 +3767,13 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="C62" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -3787,35 +3792,17 @@
       </c>
       <c r="I62" t="b">
         <v>0</v>
-      </c>
-      <c r="J62" t="s">
-        <v>118</v>
-      </c>
-      <c r="K62" t="s">
-        <v>153</v>
-      </c>
-      <c r="L62" t="s">
-        <v>142</v>
-      </c>
-      <c r="M62" t="s">
-        <v>106</v>
-      </c>
-      <c r="N62" t="s">
-        <v>156</v>
-      </c>
-      <c r="O62" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B63" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C63" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -3834,64 +3821,64 @@
       </c>
       <c r="I63" t="b">
         <v>0</v>
-      </c>
-      <c r="J63" t="s">
-        <v>118</v>
-      </c>
-      <c r="K63" t="s">
-        <v>154</v>
-      </c>
-      <c r="L63" t="s">
-        <v>144</v>
-      </c>
-      <c r="M63" t="s">
-        <v>106</v>
-      </c>
-      <c r="N63" t="s">
-        <v>155</v>
-      </c>
-      <c r="O63" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B64" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C64" t="s">
+        <v>134</v>
+      </c>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" t="b">
+        <v>0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>114</v>
+      </c>
+      <c r="K64" t="s">
+        <v>149</v>
+      </c>
+      <c r="L64" t="s">
         <v>138</v>
       </c>
-      <c r="D64" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" t="b">
-        <v>0</v>
-      </c>
-      <c r="G64" t="b">
-        <v>0</v>
-      </c>
-      <c r="H64" t="b">
-        <v>1</v>
-      </c>
-      <c r="I64" t="b">
-        <v>0</v>
+      <c r="M64" t="s">
+        <v>102</v>
+      </c>
+      <c r="N64" t="s">
+        <v>152</v>
+      </c>
+      <c r="O64" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B65" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C65" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -3910,17 +3897,35 @@
       </c>
       <c r="I65" t="b">
         <v>0</v>
+      </c>
+      <c r="J65" t="s">
+        <v>114</v>
+      </c>
+      <c r="K65" t="s">
+        <v>150</v>
+      </c>
+      <c r="L65" t="s">
+        <v>140</v>
+      </c>
+      <c r="M65" t="s">
+        <v>102</v>
+      </c>
+      <c r="N65" t="s">
+        <v>151</v>
+      </c>
+      <c r="O65" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B66" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C66" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -3943,13 +3948,13 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>143</v>
       </c>
       <c r="B67" t="s">
-        <v>185</v>
+        <v>144</v>
       </c>
       <c r="C67" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -3961,42 +3966,24 @@
         <v>0</v>
       </c>
       <c r="G67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" t="b">
         <v>0</v>
-      </c>
-      <c r="J67" t="s">
-        <v>118</v>
-      </c>
-      <c r="K67" t="s">
-        <v>152</v>
-      </c>
-      <c r="L67" t="s">
-        <v>185</v>
-      </c>
-      <c r="M67" t="s">
-        <v>106</v>
-      </c>
-      <c r="N67" t="s">
-        <v>1</v>
-      </c>
-      <c r="O67" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C68" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -4008,10 +3995,10 @@
         <v>0</v>
       </c>
       <c r="G68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" t="b">
         <v>0</v>
@@ -4019,13 +4006,13 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>49</v>
       </c>
       <c r="B69" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="C69" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -4046,33 +4033,33 @@
         <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K69" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="L69" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="M69" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="N69" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="O69" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C70" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -4091,35 +4078,17 @@
       </c>
       <c r="I70" t="b">
         <v>0</v>
-      </c>
-      <c r="J70" t="s">
-        <v>118</v>
-      </c>
-      <c r="K70" t="s">
-        <v>154</v>
-      </c>
-      <c r="L70" t="s">
-        <v>144</v>
-      </c>
-      <c r="M70" t="s">
-        <v>106</v>
-      </c>
-      <c r="N70" t="s">
-        <v>155</v>
-      </c>
-      <c r="O70" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C71" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -4138,17 +4107,35 @@
       </c>
       <c r="I71" t="b">
         <v>0</v>
+      </c>
+      <c r="J71" t="s">
+        <v>114</v>
+      </c>
+      <c r="K71" t="s">
+        <v>149</v>
+      </c>
+      <c r="L71" t="s">
+        <v>138</v>
+      </c>
+      <c r="M71" t="s">
+        <v>102</v>
+      </c>
+      <c r="N71" t="s">
+        <v>152</v>
+      </c>
+      <c r="O71" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B72" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C72" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -4167,17 +4154,35 @@
       </c>
       <c r="I72" t="b">
         <v>0</v>
+      </c>
+      <c r="J72" t="s">
+        <v>114</v>
+      </c>
+      <c r="K72" t="s">
+        <v>150</v>
+      </c>
+      <c r="L72" t="s">
+        <v>140</v>
+      </c>
+      <c r="M72" t="s">
+        <v>102</v>
+      </c>
+      <c r="N72" t="s">
+        <v>151</v>
+      </c>
+      <c r="O72" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C73" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -4198,10 +4203,68 @@
         <v>0</v>
       </c>
     </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>143</v>
+      </c>
+      <c r="B74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C74" t="s">
+        <v>180</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" t="b">
+        <v>1</v>
+      </c>
+      <c r="H74" t="b">
+        <v>0</v>
+      </c>
+      <c r="I74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" t="s">
+        <v>146</v>
+      </c>
+      <c r="C75" t="s">
+        <v>180</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="G75" t="b">
+        <v>1</v>
+      </c>
+      <c r="H75" t="b">
+        <v>0</v>
+      </c>
+      <c r="I75" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O73" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}"/>
+  <autoFilter ref="A1:O75" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}"/>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D1:I1 H2:I2 G2:G16 D2:F57 H3:H57 I3:I73 G20:G34 G38:G52 G56:G57 D58:H58 D59:F68 H59:H68 G59:G73">
+  <conditionalFormatting sqref="D1:I1 G19:G33 G58:G59 D60:H60 D61:F70 H61:H70 G61:G75 G9:G15 D53:F59 G53:G54 G37:G50 I53:I75 H9:I50 H53:H59 D51:I52 G2:I8 D2:F50">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add new functions for focal area and landowner data processing, enhance UI components, and update database interactions 🌱✨
- Implemented `focal_area_from_prop_name` function to retrieve focal areas based on property names from the database.
- Enhanced `prep_view_landowners` function to include property names associated with landowners.
- Updated `prep_view_pid` to support multiple selected views for PID data.
- Created `prep_view_query_focal_area` function to query focal area data and integrate it with existing data processing.
- Refactored `module_action_item_tracking` and `module_data_viewer` to improve UI and server logic, including the addition of reactive elements for securement notes.
- Modified `module_outreach_queries` to streamline query selection and data retrieval processes.
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="450" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC35E329-B45F-4E52-908C-B8EAC05D5359}"/>
+  <xr:revisionPtr revIDLastSave="464" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D299D014-3F05-4295-A144-AB1D5587D829}"/>
   <bookViews>
-    <workbookView xWindow="-192" yWindow="-192" windowWidth="23424" windowHeight="12624" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">names!$A$1:$O$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">names!$A$1:$P$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="193">
   <si>
     <t>db_name</t>
   </si>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>Size (acres) Confirmed</t>
+  </si>
+  <si>
+    <t>pid_view_04</t>
   </si>
 </sst>
 </file>
@@ -1468,11 +1471,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}">
-  <dimension ref="A1:O75"/>
+  <dimension ref="A1:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1481,18 +1484,19 @@
     <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.796875" customWidth="1"/>
     <col min="4" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.59765625" customWidth="1"/>
-    <col min="9" max="9" width="18.09765625" customWidth="1"/>
-    <col min="10" max="10" width="9.19921875" customWidth="1"/>
-    <col min="11" max="11" width="15.8984375" customWidth="1"/>
-    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.59765625" customWidth="1"/>
+    <col min="10" max="10" width="18.09765625" customWidth="1"/>
+    <col min="11" max="11" width="9.19921875" customWidth="1"/>
+    <col min="12" max="12" width="15.8984375" customWidth="1"/>
+    <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -1512,34 +1516,37 @@
         <v>184</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1558,17 +1565,20 @@
       <c r="F2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G2" t="b">
+      <c r="G2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1588,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -1596,8 +1606,11 @@
       <c r="I3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1617,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -1625,8 +1638,11 @@
       <c r="I4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1646,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -1654,26 +1670,29 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
         <v>114</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>100</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>4</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>102</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>103</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1701,8 +1720,11 @@
       <c r="I6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1722,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -1730,26 +1752,29 @@
       <c r="I7" t="b">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
         <v>114</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>105</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>6</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>102</v>
-      </c>
-      <c r="N7" t="s">
-        <v>106</v>
       </c>
       <c r="O7" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>186</v>
       </c>
@@ -1769,7 +1794,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -1777,8 +1802,11 @@
       <c r="I8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1798,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -1806,26 +1834,29 @@
       <c r="I9" t="b">
         <v>0</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
         <v>114</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>107</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>7</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>102</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>108</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1853,8 +1884,11 @@
       <c r="I10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -1882,8 +1916,11 @@
       <c r="I11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -1903,7 +1940,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -1911,26 +1948,29 @@
       <c r="I12" t="b">
         <v>0</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
         <v>114</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>109</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>10</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>102</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>110</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1950,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -1958,26 +1998,29 @@
       <c r="I13" t="b">
         <v>0</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
         <v>114</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>109</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>11</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>102</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>110</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1997,7 +2040,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -2005,26 +2048,29 @@
       <c r="I14" t="b">
         <v>0</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
         <v>114</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>109</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>12</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>102</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>110</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -2050,28 +2096,31 @@
         <v>0</v>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
         <v>114</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>156</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>13</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>102</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>157</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -2097,28 +2146,31 @@
         <v>0</v>
       </c>
       <c r="I16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
         <v>114</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>156</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>46</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>102</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>157</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -2144,28 +2196,31 @@
         <v>0</v>
       </c>
       <c r="I17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
         <v>114</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>156</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>14</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>102</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>157</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -2191,28 +2246,31 @@
         <v>0</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
         <v>114</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>156</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>15</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>102</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>157</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -2238,28 +2296,31 @@
         <v>0</v>
       </c>
       <c r="I19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
         <v>114</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>156</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>16</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>102</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>157</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -2285,28 +2346,31 @@
         <v>0</v>
       </c>
       <c r="I20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
         <v>114</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>156</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>17</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>102</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>157</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -2332,28 +2396,31 @@
         <v>0</v>
       </c>
       <c r="I21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
         <v>114</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>156</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>18</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>102</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>157</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -2379,28 +2446,31 @@
         <v>0</v>
       </c>
       <c r="I22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
         <v>114</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>156</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>19</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>102</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>157</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -2428,8 +2498,11 @@
       <c r="I23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -2457,8 +2530,11 @@
       <c r="I24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -2484,28 +2560,31 @@
         <v>0</v>
       </c>
       <c r="I25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
         <v>114</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>156</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>22</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>102</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>157</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -2531,28 +2610,31 @@
         <v>0</v>
       </c>
       <c r="I26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
         <v>114</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>156</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>23</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>102</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>157</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -2578,28 +2660,31 @@
         <v>0</v>
       </c>
       <c r="I27" t="b">
-        <v>1</v>
-      </c>
-      <c r="J27" t="s">
+        <v>0</v>
+      </c>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
         <v>114</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>156</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>24</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>102</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>157</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2625,28 +2710,31 @@
         <v>0</v>
       </c>
       <c r="I28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" t="s">
+        <v>0</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
         <v>114</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>156</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>25</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>102</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>157</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -2672,28 +2760,31 @@
         <v>0</v>
       </c>
       <c r="I29" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
         <v>114</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>156</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>26</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>102</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>157</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2719,28 +2810,31 @@
         <v>0</v>
       </c>
       <c r="I30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
         <v>114</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>156</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>27</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>102</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>157</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -2768,8 +2862,11 @@
       <c r="I31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -2795,28 +2892,31 @@
         <v>0</v>
       </c>
       <c r="I32" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
         <v>114</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>156</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>29</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>102</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>157</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2842,28 +2942,31 @@
         <v>0</v>
       </c>
       <c r="I33" t="b">
-        <v>1</v>
-      </c>
-      <c r="J33" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="s">
         <v>114</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>156</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>30</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>102</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>157</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -2889,28 +2992,31 @@
         <v>0</v>
       </c>
       <c r="I34" t="b">
-        <v>1</v>
-      </c>
-      <c r="J34" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
         <v>114</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>156</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>31</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>102</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>157</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -2936,28 +3042,31 @@
         <v>0</v>
       </c>
       <c r="I35" t="b">
-        <v>1</v>
-      </c>
-      <c r="J35" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
         <v>114</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>156</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>32</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>102</v>
       </c>
-      <c r="N35" t="s">
+      <c r="O35" t="s">
         <v>157</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -2983,28 +3092,31 @@
         <v>0</v>
       </c>
       <c r="I36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J36" t="s">
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
         <v>114</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>156</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>33</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>102</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
         <v>157</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -3030,28 +3142,31 @@
         <v>0</v>
       </c>
       <c r="I37" t="b">
-        <v>1</v>
-      </c>
-      <c r="J37" t="s">
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
         <v>114</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>156</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>34</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>102</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>157</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -3079,26 +3194,29 @@
       <c r="I38" t="b">
         <v>0</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
         <v>114</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>156</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
         <v>47</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>102</v>
       </c>
-      <c r="N38" t="s">
+      <c r="O38" t="s">
         <v>157</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>189</v>
       </c>
@@ -3126,8 +3244,11 @@
       <c r="I39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -3155,8 +3276,11 @@
       <c r="I40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -3184,8 +3308,11 @@
       <c r="I41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -3205,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="b">
         <v>0</v>
@@ -3213,8 +3340,11 @@
       <c r="I42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -3242,8 +3372,11 @@
       <c r="I43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -3271,8 +3404,11 @@
       <c r="I44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -3300,8 +3436,11 @@
       <c r="I45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -3329,8 +3468,11 @@
       <c r="I46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -3358,8 +3500,11 @@
       <c r="I47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -3387,8 +3532,11 @@
       <c r="I48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -3416,8 +3564,11 @@
       <c r="I49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -3445,8 +3596,11 @@
       <c r="I50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>135</v>
       </c>
@@ -3474,8 +3628,11 @@
       <c r="I51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>191</v>
       </c>
@@ -3503,8 +3660,11 @@
       <c r="I52" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>118</v>
       </c>
@@ -3532,8 +3692,11 @@
       <c r="I53" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>120</v>
       </c>
@@ -3561,8 +3724,11 @@
       <c r="I54" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>122</v>
       </c>
@@ -3590,8 +3756,11 @@
       <c r="I55" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>124</v>
       </c>
@@ -3619,8 +3788,11 @@
       <c r="I56" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>126</v>
       </c>
@@ -3648,8 +3820,11 @@
       <c r="I57" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>128</v>
       </c>
@@ -3677,8 +3852,11 @@
       <c r="I58" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>130</v>
       </c>
@@ -3706,8 +3884,11 @@
       <c r="I59" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>143</v>
       </c>
@@ -3735,8 +3916,11 @@
       <c r="I60" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>132</v>
       </c>
@@ -3764,8 +3948,11 @@
       <c r="I61" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>118</v>
       </c>
@@ -3788,13 +3975,16 @@
         <v>0</v>
       </c>
       <c r="H62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>135</v>
       </c>
@@ -3817,13 +4007,16 @@
         <v>0</v>
       </c>
       <c r="H63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>137</v>
       </c>
@@ -3846,31 +4039,34 @@
         <v>0</v>
       </c>
       <c r="H64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" t="b">
-        <v>0</v>
-      </c>
-      <c r="J64" t="s">
+        <v>1</v>
+      </c>
+      <c r="J64" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" t="s">
         <v>114</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>149</v>
       </c>
-      <c r="L64" t="s">
+      <c r="M64" t="s">
         <v>138</v>
       </c>
-      <c r="M64" t="s">
+      <c r="N64" t="s">
         <v>102</v>
       </c>
-      <c r="N64" t="s">
+      <c r="O64" t="s">
         <v>152</v>
       </c>
-      <c r="O64" t="s">
+      <c r="P64" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>139</v>
       </c>
@@ -3893,31 +4089,34 @@
         <v>0</v>
       </c>
       <c r="H65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="b">
-        <v>0</v>
-      </c>
-      <c r="J65" t="s">
+        <v>1</v>
+      </c>
+      <c r="J65" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" t="s">
         <v>114</v>
       </c>
-      <c r="K65" t="s">
+      <c r="L65" t="s">
         <v>150</v>
       </c>
-      <c r="L65" t="s">
+      <c r="M65" t="s">
         <v>140</v>
       </c>
-      <c r="M65" t="s">
+      <c r="N65" t="s">
         <v>102</v>
       </c>
-      <c r="N65" t="s">
+      <c r="O65" t="s">
         <v>151</v>
       </c>
-      <c r="O65" t="s">
+      <c r="P65" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>141</v>
       </c>
@@ -3940,13 +4139,16 @@
         <v>0</v>
       </c>
       <c r="H66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>143</v>
       </c>
@@ -3969,13 +4171,16 @@
         <v>0</v>
       </c>
       <c r="H67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>145</v>
       </c>
@@ -3998,13 +4203,16 @@
         <v>0</v>
       </c>
       <c r="H68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>49</v>
       </c>
@@ -4024,34 +4232,37 @@
         <v>0</v>
       </c>
       <c r="G69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69" t="b">
         <v>0</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J69" t="b">
+        <v>0</v>
+      </c>
+      <c r="K69" t="s">
         <v>114</v>
       </c>
-      <c r="K69" t="s">
-        <v>148</v>
-      </c>
       <c r="L69" t="s">
+        <v>148</v>
+      </c>
+      <c r="M69" t="s">
         <v>181</v>
       </c>
-      <c r="M69" t="s">
+      <c r="N69" t="s">
         <v>102</v>
       </c>
-      <c r="N69" t="s">
-        <v>1</v>
-      </c>
       <c r="O69" t="s">
+        <v>1</v>
+      </c>
+      <c r="P69" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>132</v>
       </c>
@@ -4071,16 +4282,19 @@
         <v>0</v>
       </c>
       <c r="G70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>137</v>
       </c>
@@ -4100,34 +4314,37 @@
         <v>0</v>
       </c>
       <c r="G71" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71" t="b">
         <v>0</v>
       </c>
-      <c r="J71" t="s">
+      <c r="J71" t="b">
+        <v>0</v>
+      </c>
+      <c r="K71" t="s">
         <v>114</v>
       </c>
-      <c r="K71" t="s">
+      <c r="L71" t="s">
         <v>149</v>
       </c>
-      <c r="L71" t="s">
+      <c r="M71" t="s">
         <v>138</v>
       </c>
-      <c r="M71" t="s">
+      <c r="N71" t="s">
         <v>102</v>
       </c>
-      <c r="N71" t="s">
+      <c r="O71" t="s">
         <v>152</v>
       </c>
-      <c r="O71" t="s">
+      <c r="P71" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>139</v>
       </c>
@@ -4147,34 +4364,37 @@
         <v>0</v>
       </c>
       <c r="G72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" t="b">
         <v>0</v>
       </c>
-      <c r="J72" t="s">
+      <c r="J72" t="b">
+        <v>0</v>
+      </c>
+      <c r="K72" t="s">
         <v>114</v>
       </c>
-      <c r="K72" t="s">
+      <c r="L72" t="s">
         <v>150</v>
       </c>
-      <c r="L72" t="s">
+      <c r="M72" t="s">
         <v>140</v>
       </c>
-      <c r="M72" t="s">
+      <c r="N72" t="s">
         <v>102</v>
       </c>
-      <c r="N72" t="s">
+      <c r="O72" t="s">
         <v>151</v>
       </c>
-      <c r="O72" t="s">
+      <c r="P72" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>141</v>
       </c>
@@ -4194,16 +4414,19 @@
         <v>0</v>
       </c>
       <c r="G73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -4223,16 +4446,19 @@
         <v>0</v>
       </c>
       <c r="G74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>145</v>
       </c>
@@ -4252,19 +4478,22 @@
         <v>0</v>
       </c>
       <c r="G75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75" t="b">
         <v>0</v>
       </c>
+      <c r="J75" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O75" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}"/>
+  <autoFilter ref="A1:P75" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}"/>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D1:I1 G19:G33 G58:G59 D60:H60 D61:F70 H61:H70 G61:G75 G9:G15 D53:F59 G53:G54 G37:G50 I53:I75 H9:I50 H53:H59 D51:I52 G2:I8 D2:F50">
+  <conditionalFormatting sqref="D1:J1 H2:J8 D2:G70 H9:H15 I9:J50 H19:H33 H37:H50 H51:J52 H53:H54 I53:I59 J53:J75 H58:H59 H60:I60 I61:I70 H61:H75">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Refactored server code in order to make things compatible with the updated database schema. Added popup functionality.
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="516" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE194E7D-C6A9-4907-A599-88588EC02537}"/>
+  <xr:revisionPtr revIDLastSave="522" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9BA9ECF-468F-4DFF-B0F5-191448FC3551}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="210">
   <si>
     <t>db_name</t>
   </si>
@@ -657,6 +657,15 @@
   </si>
   <si>
     <t>Environmental Investigation</t>
+  </si>
+  <si>
+    <t>Landowner Description</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>County</t>
   </si>
 </sst>
 </file>
@@ -1513,11 +1522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1795,16 +1804,16 @@
         <v>147</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
       <c r="F7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -1848,16 +1857,16 @@
         <v>147</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -4180,7 +4189,7 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>142</v>
+        <v>207</v>
       </c>
       <c r="B61" t="s">
         <v>182</v>
@@ -4866,6 +4875,14 @@
       </c>
       <c r="B81" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>209</v>
+      </c>
+      <c r="B82" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major refactor: moving from "landowner" to "property contact" in database schema and UI.
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="522" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9BA9ECF-468F-4DFF-B0F5-191448FC3551}"/>
+  <xr:revisionPtr revIDLastSave="538" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F0AD360-4B8B-46CD-A172-69BAF142E2E3}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="212">
   <si>
     <t>db_name</t>
   </si>
@@ -392,9 +392,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>landowner_contact_details</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -425,21 +422,12 @@
     <t>phone_cell</t>
   </si>
   <si>
-    <t>Landowner PIDs</t>
-  </si>
-  <si>
-    <t>landowner_pids</t>
-  </si>
-  <si>
     <t>DNC</t>
   </si>
   <si>
     <t>dnc</t>
   </si>
   <si>
-    <t>landowner_communication</t>
-  </si>
-  <si>
     <t>Landowner Contact ID</t>
   </si>
   <si>
@@ -584,9 +572,6 @@
     <t>parcel_value</t>
   </si>
   <si>
-    <t>landowner_description</t>
-  </si>
-  <si>
     <t>pid_view_03</t>
   </si>
   <si>
@@ -659,20 +644,41 @@
     <t>Environmental Investigation</t>
   </si>
   <si>
-    <t>Landowner Description</t>
-  </si>
-  <si>
     <t>county</t>
   </si>
   <si>
     <t>County</t>
+  </si>
+  <si>
+    <t>property_contact_id</t>
+  </si>
+  <si>
+    <t>Property Contact ID</t>
+  </si>
+  <si>
+    <t>property_contact_communication</t>
+  </si>
+  <si>
+    <t>property_contact_details</t>
+  </si>
+  <si>
+    <t>Property Contact Description</t>
+  </si>
+  <si>
+    <t>property_contact_description</t>
+  </si>
+  <si>
+    <t>property_contact_pids</t>
+  </si>
+  <si>
+    <t>Property Contact PIDs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -792,6 +798,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Aptos"/>
       <family val="2"/>
     </font>
@@ -1137,9 +1149,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1525,13 +1538,13 @@
   <dimension ref="A1:Q82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7:F8"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.796875" customWidth="1"/>
     <col min="4" max="6" width="13" bestFit="1" customWidth="1"/>
@@ -1555,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>115</v>
@@ -1564,22 +1577,22 @@
         <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>113</v>
@@ -1608,7 +1621,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D2" s="1" t="b">
         <v>1</v>
@@ -1643,7 +1656,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1678,7 +1691,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1713,7 +1726,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -1766,7 +1779,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1801,7 +1814,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -1848,13 +1861,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1886,7 +1899,7 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
         <v>99</v>
@@ -1922,7 +1935,7 @@
         <v>106</v>
       </c>
       <c r="N9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="O9" t="s">
         <v>101</v>
@@ -1931,7 +1944,7 @@
         <v>107</v>
       </c>
       <c r="Q9" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1942,7 +1955,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -1995,7 +2008,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -2030,7 +2043,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -2065,7 +2078,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -2118,7 +2131,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -2171,7 +2184,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -2224,7 +2237,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -2254,7 +2267,7 @@
         <v>113</v>
       </c>
       <c r="M16" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N16" t="s">
         <v>13</v>
@@ -2263,10 +2276,10 @@
         <v>101</v>
       </c>
       <c r="P16" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q16" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
@@ -2277,7 +2290,7 @@
         <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -2307,7 +2320,7 @@
         <v>113</v>
       </c>
       <c r="M17" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N17" t="s">
         <v>46</v>
@@ -2316,10 +2329,10 @@
         <v>101</v>
       </c>
       <c r="P17" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
@@ -2330,7 +2343,7 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -2360,7 +2373,7 @@
         <v>113</v>
       </c>
       <c r="M18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N18" t="s">
         <v>14</v>
@@ -2369,10 +2382,10 @@
         <v>101</v>
       </c>
       <c r="P18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q18" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
@@ -2383,7 +2396,7 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -2413,7 +2426,7 @@
         <v>113</v>
       </c>
       <c r="M19" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N19" t="s">
         <v>15</v>
@@ -2422,10 +2435,10 @@
         <v>101</v>
       </c>
       <c r="P19" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q19" t="s">
         <v>156</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -2436,7 +2449,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -2466,7 +2479,7 @@
         <v>113</v>
       </c>
       <c r="M20" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N20" t="s">
         <v>16</v>
@@ -2475,21 +2488,21 @@
         <v>101</v>
       </c>
       <c r="P20" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q20" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -2519,7 +2532,7 @@
         <v>113</v>
       </c>
       <c r="M21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N21" t="s">
         <v>17</v>
@@ -2528,10 +2541,10 @@
         <v>101</v>
       </c>
       <c r="P21" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -2542,7 +2555,7 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -2572,7 +2585,7 @@
         <v>113</v>
       </c>
       <c r="M22" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N22" t="s">
         <v>18</v>
@@ -2581,10 +2594,10 @@
         <v>101</v>
       </c>
       <c r="P22" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q22" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
@@ -2595,7 +2608,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -2625,7 +2638,7 @@
         <v>113</v>
       </c>
       <c r="M23" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N23" t="s">
         <v>19</v>
@@ -2634,10 +2647,10 @@
         <v>101</v>
       </c>
       <c r="P23" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q23" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
@@ -2648,7 +2661,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -2683,7 +2696,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -2718,7 +2731,7 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -2748,7 +2761,7 @@
         <v>113</v>
       </c>
       <c r="M26" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N26" t="s">
         <v>22</v>
@@ -2757,10 +2770,10 @@
         <v>101</v>
       </c>
       <c r="P26" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q26" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
@@ -2771,7 +2784,7 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -2801,7 +2814,7 @@
         <v>113</v>
       </c>
       <c r="M27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N27" t="s">
         <v>23</v>
@@ -2810,10 +2823,10 @@
         <v>101</v>
       </c>
       <c r="P27" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q27" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
@@ -2824,7 +2837,7 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -2854,7 +2867,7 @@
         <v>113</v>
       </c>
       <c r="M28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N28" t="s">
         <v>24</v>
@@ -2863,10 +2876,10 @@
         <v>101</v>
       </c>
       <c r="P28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q28" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
@@ -2877,7 +2890,7 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D29" t="b">
         <v>0</v>
@@ -2907,7 +2920,7 @@
         <v>113</v>
       </c>
       <c r="M29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N29" t="s">
         <v>25</v>
@@ -2916,10 +2929,10 @@
         <v>101</v>
       </c>
       <c r="P29" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q29" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
@@ -2930,7 +2943,7 @@
         <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -2960,7 +2973,7 @@
         <v>113</v>
       </c>
       <c r="M30" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N30" t="s">
         <v>26</v>
@@ -2969,10 +2982,10 @@
         <v>101</v>
       </c>
       <c r="P30" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q30" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
@@ -2983,7 +2996,7 @@
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
@@ -3013,7 +3026,7 @@
         <v>113</v>
       </c>
       <c r="M31" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N31" t="s">
         <v>27</v>
@@ -3022,10 +3035,10 @@
         <v>101</v>
       </c>
       <c r="P31" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q31" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
@@ -3036,7 +3049,7 @@
         <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -3071,7 +3084,7 @@
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -3101,7 +3114,7 @@
         <v>113</v>
       </c>
       <c r="M33" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N33" t="s">
         <v>29</v>
@@ -3110,10 +3123,10 @@
         <v>101</v>
       </c>
       <c r="P33" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q33" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
@@ -3124,7 +3137,7 @@
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -3154,7 +3167,7 @@
         <v>113</v>
       </c>
       <c r="M34" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N34" t="s">
         <v>30</v>
@@ -3163,10 +3176,10 @@
         <v>101</v>
       </c>
       <c r="P34" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q34" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
@@ -3177,7 +3190,7 @@
         <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -3207,7 +3220,7 @@
         <v>113</v>
       </c>
       <c r="M35" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N35" t="s">
         <v>31</v>
@@ -3216,10 +3229,10 @@
         <v>101</v>
       </c>
       <c r="P35" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q35" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
@@ -3230,7 +3243,7 @@
         <v>32</v>
       </c>
       <c r="C36" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
@@ -3260,7 +3273,7 @@
         <v>113</v>
       </c>
       <c r="M36" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N36" t="s">
         <v>32</v>
@@ -3269,10 +3282,10 @@
         <v>101</v>
       </c>
       <c r="P36" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q36" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
@@ -3283,7 +3296,7 @@
         <v>33</v>
       </c>
       <c r="C37" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
@@ -3313,7 +3326,7 @@
         <v>113</v>
       </c>
       <c r="M37" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N37" t="s">
         <v>33</v>
@@ -3322,10 +3335,10 @@
         <v>101</v>
       </c>
       <c r="P37" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q37" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
@@ -3336,7 +3349,7 @@
         <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
@@ -3366,7 +3379,7 @@
         <v>113</v>
       </c>
       <c r="M38" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N38" t="s">
         <v>34</v>
@@ -3375,10 +3388,10 @@
         <v>101</v>
       </c>
       <c r="P38" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q38" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
@@ -3389,7 +3402,7 @@
         <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D39" t="b">
         <v>0</v>
@@ -3419,7 +3432,7 @@
         <v>113</v>
       </c>
       <c r="M39" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="N39" t="s">
         <v>47</v>
@@ -3428,21 +3441,21 @@
         <v>101</v>
       </c>
       <c r="P39" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="Q39" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B40" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -3477,7 +3490,7 @@
         <v>35</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
@@ -3512,7 +3525,7 @@
         <v>36</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
@@ -3547,7 +3560,7 @@
         <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D43" t="b">
         <v>0</v>
@@ -3582,7 +3595,7 @@
         <v>38</v>
       </c>
       <c r="C44" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -3617,7 +3630,7 @@
         <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -3652,7 +3665,7 @@
         <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -3687,7 +3700,7 @@
         <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
@@ -3722,7 +3735,7 @@
         <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D48" t="b">
         <v>0</v>
@@ -3757,7 +3770,7 @@
         <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D49" t="b">
         <v>0</v>
@@ -3792,7 +3805,7 @@
         <v>44</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
@@ -3822,7 +3835,7 @@
         <v>113</v>
       </c>
       <c r="M50" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="N50" t="s">
         <v>44</v>
@@ -3831,10 +3844,10 @@
         <v>101</v>
       </c>
       <c r="P50" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="Q50" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
@@ -3845,7 +3858,7 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
@@ -3874,13 +3887,13 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
@@ -3909,13 +3922,13 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B53" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C53" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
@@ -3950,7 +3963,7 @@
         <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -3979,13 +3992,13 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" t="s">
         <v>119</v>
       </c>
-      <c r="B55" t="s">
-        <v>120</v>
-      </c>
       <c r="C55" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -4014,13 +4027,13 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
         <v>121</v>
       </c>
-      <c r="B56" t="s">
-        <v>122</v>
-      </c>
       <c r="C56" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -4049,13 +4062,13 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" t="s">
         <v>123</v>
       </c>
-      <c r="B57" t="s">
-        <v>124</v>
-      </c>
       <c r="C57" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -4084,13 +4097,13 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" t="s">
         <v>125</v>
       </c>
-      <c r="B58" t="s">
-        <v>126</v>
-      </c>
       <c r="C58" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -4119,13 +4132,13 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" t="s">
         <v>127</v>
       </c>
-      <c r="B59" t="s">
-        <v>128</v>
-      </c>
       <c r="C59" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -4154,13 +4167,13 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>211</v>
       </c>
       <c r="B60" t="s">
-        <v>130</v>
+        <v>210</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -4186,16 +4199,17 @@
       <c r="K60" t="b">
         <v>0</v>
       </c>
+      <c r="L60" s="2"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>208</v>
+      </c>
+      <c r="B61" t="s">
+        <v>209</v>
+      </c>
+      <c r="C61" t="s">
         <v>207</v>
-      </c>
-      <c r="B61" t="s">
-        <v>182</v>
-      </c>
-      <c r="C61" t="s">
-        <v>118</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -4224,13 +4238,13 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>207</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -4265,7 +4279,7 @@
         <v>101</v>
       </c>
       <c r="C63" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -4294,13 +4308,13 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>205</v>
       </c>
       <c r="B64" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="C64" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -4329,13 +4343,13 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B65" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C65" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -4365,30 +4379,30 @@
         <v>113</v>
       </c>
       <c r="M65" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N65" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O65" t="s">
         <v>101</v>
       </c>
       <c r="P65" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q65" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B66" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -4418,30 +4432,30 @@
         <v>113</v>
       </c>
       <c r="M66" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="N66" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O66" t="s">
         <v>101</v>
       </c>
       <c r="P66" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="Q66" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B67" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -4470,13 +4484,13 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C68" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -4505,13 +4519,13 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C69" t="s">
-        <v>133</v>
+        <v>206</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -4543,10 +4557,10 @@
         <v>49</v>
       </c>
       <c r="B70" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C70" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
@@ -4576,10 +4590,10 @@
         <v>113</v>
       </c>
       <c r="M70" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="N70" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="O70" t="s">
         <v>101</v>
@@ -4588,18 +4602,18 @@
         <v>1</v>
       </c>
       <c r="Q70" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C71" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
@@ -4628,13 +4642,13 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C72" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
@@ -4664,30 +4678,30 @@
         <v>113</v>
       </c>
       <c r="M72" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N72" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O72" t="s">
         <v>101</v>
       </c>
       <c r="P72" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q72" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C73" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
@@ -4717,30 +4731,30 @@
         <v>113</v>
       </c>
       <c r="M73" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="N73" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O73" t="s">
         <v>101</v>
       </c>
       <c r="P73" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="Q73" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B74" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C74" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -4769,13 +4783,13 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B75" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C75" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -4804,13 +4818,13 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C76" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D76" t="b">
         <v>0</v>
@@ -4842,53 +4856,53 @@
         <v>54</v>
       </c>
       <c r="B77" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B78" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B79" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B80" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B81" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B82" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q76" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}"/>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D1:K1 H2:K9 D2:G71 H10:H16 I10:K51 H20:H34 H38:H51 H52:K53 H54:H55 I54:I60 J54:K76 H59:H60 H61:I61 I62:I71 H62:H76">
+  <conditionalFormatting sqref="D1:K1 H2:K9 D2:G59 H10:H16 I10:K51 H20:H34 H38:H51 H52:K53 H54:H55 I54:K59 H59 H61:I61 I62:I71 H62:H76 J61:K76 D61:G71">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Bug fixes and refactoring database attribute names
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="538" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F0AD360-4B8B-46CD-A172-69BAF142E2E3}"/>
+  <xr:revisionPtr revIDLastSave="540" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48B7C3BA-E6BE-4FF2-A542-EB42A715C92F}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
@@ -584,12 +584,6 @@
     <t>phase_id_description</t>
   </si>
   <si>
-    <t>securement_action_notes</t>
-  </si>
-  <si>
-    <t>Securement Action Notes</t>
-  </si>
-  <si>
     <t>size_acres_confirmed</t>
   </si>
   <si>
@@ -672,6 +666,12 @@
   </si>
   <si>
     <t>Property Contact PIDs</t>
+  </si>
+  <si>
+    <t>securement_action_description</t>
+  </si>
+  <si>
+    <t>Securement Action Description</t>
   </si>
 </sst>
 </file>
@@ -1538,8 +1538,8 @@
   <dimension ref="A1:Q82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1580,7 +1580,7 @@
         <v>178</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>174</v>
@@ -1592,7 +1592,7 @@
         <v>179</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>113</v>
@@ -1899,7 +1899,7 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C9" t="s">
         <v>99</v>
@@ -1935,7 +1935,7 @@
         <v>106</v>
       </c>
       <c r="N9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O9" t="s">
         <v>101</v>
@@ -1944,7 +1944,7 @@
         <v>107</v>
       </c>
       <c r="Q9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -2496,7 +2496,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -3449,10 +3449,10 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="B40" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="C40" t="s">
         <v>143</v>
@@ -3835,7 +3835,7 @@
         <v>113</v>
       </c>
       <c r="M50" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N50" t="s">
         <v>44</v>
@@ -3844,10 +3844,10 @@
         <v>101</v>
       </c>
       <c r="P50" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="Q50" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
@@ -3922,10 +3922,10 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B53" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C53" t="s">
         <v>143</v>
@@ -3963,7 +3963,7 @@
         <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -3998,7 +3998,7 @@
         <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -4033,7 +4033,7 @@
         <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -4068,7 +4068,7 @@
         <v>123</v>
       </c>
       <c r="C57" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -4103,7 +4103,7 @@
         <v>125</v>
       </c>
       <c r="C58" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -4138,7 +4138,7 @@
         <v>127</v>
       </c>
       <c r="C59" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -4167,13 +4167,13 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B60" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C60" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -4203,13 +4203,13 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B61" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C61" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -4244,7 +4244,7 @@
         <v>129</v>
       </c>
       <c r="C62" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -4279,7 +4279,7 @@
         <v>101</v>
       </c>
       <c r="C63" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -4308,13 +4308,13 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B64" t="s">
+        <v>202</v>
+      </c>
+      <c r="C64" t="s">
         <v>204</v>
-      </c>
-      <c r="C64" t="s">
-        <v>206</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -4349,7 +4349,7 @@
         <v>133</v>
       </c>
       <c r="C65" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -4402,7 +4402,7 @@
         <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -4455,7 +4455,7 @@
         <v>137</v>
       </c>
       <c r="C67" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -4490,7 +4490,7 @@
         <v>139</v>
       </c>
       <c r="C68" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -4525,7 +4525,7 @@
         <v>141</v>
       </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -4856,53 +4856,53 @@
         <v>54</v>
       </c>
       <c r="B77" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B78" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B79" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B80" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B81" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B82" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q76" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}"/>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D1:K1 H2:K9 D2:G59 H10:H16 I10:K51 H20:H34 H38:H51 H52:K53 H54:H55 I54:K59 H59 H61:I61 I62:I71 H62:H76 J61:K76 D61:G71">
+  <conditionalFormatting sqref="D1:K1 H2:K9 D2:G59 H10:H16 I10:K51 H20:H34 H38:H51 H52:K53 H54:H55 I54:K59 H59 H61:I61 D61:G71 J61:K76 I62:I71 H62:H76">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",D1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Bump version to 2.4.5; add app_data/papa_pending.fgb to .gitignore; update df_views.xlsx
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="540" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48B7C3BA-E6BE-4FF2-A542-EB42A715C92F}"/>
+  <xr:revisionPtr revIDLastSave="543" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB999478-2925-447F-8130-FA7654D6AD5E}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="214">
   <si>
     <t>db_name</t>
   </si>
@@ -629,9 +629,6 @@
     <t>price_per_acre</t>
   </si>
   <si>
-    <t>Price per acre</t>
-  </si>
-  <si>
     <t>Focus Area (Internal)</t>
   </si>
   <si>
@@ -672,6 +669,15 @@
   </si>
   <si>
     <t>Securement Action Description</t>
+  </si>
+  <si>
+    <t>Size (ha)</t>
+  </si>
+  <si>
+    <t>size_ha</t>
+  </si>
+  <si>
+    <t>Price Per Acre</t>
   </si>
 </sst>
 </file>
@@ -1535,11 +1541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7224EA0-91C0-498C-ACC9-0DF402789E13}">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2496,7 +2502,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
@@ -3449,10 +3455,10 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C40" t="s">
         <v>143</v>
@@ -3963,7 +3969,7 @@
         <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
@@ -3998,7 +4004,7 @@
         <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
@@ -4033,7 +4039,7 @@
         <v>121</v>
       </c>
       <c r="C56" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
@@ -4068,7 +4074,7 @@
         <v>123</v>
       </c>
       <c r="C57" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D57" t="b">
         <v>0</v>
@@ -4103,7 +4109,7 @@
         <v>125</v>
       </c>
       <c r="C58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
@@ -4138,7 +4144,7 @@
         <v>127</v>
       </c>
       <c r="C59" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D59" t="b">
         <v>0</v>
@@ -4167,13 +4173,13 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
@@ -4203,13 +4209,13 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B61" t="s">
         <v>206</v>
       </c>
-      <c r="B61" t="s">
-        <v>207</v>
-      </c>
       <c r="C61" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D61" t="b">
         <v>0</v>
@@ -4244,7 +4250,7 @@
         <v>129</v>
       </c>
       <c r="C62" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -4279,7 +4285,7 @@
         <v>101</v>
       </c>
       <c r="C63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D63" t="b">
         <v>0</v>
@@ -4308,13 +4314,13 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>202</v>
+      </c>
+      <c r="B64" t="s">
+        <v>201</v>
+      </c>
+      <c r="C64" t="s">
         <v>203</v>
-      </c>
-      <c r="B64" t="s">
-        <v>202</v>
-      </c>
-      <c r="C64" t="s">
-        <v>204</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
@@ -4349,7 +4355,7 @@
         <v>133</v>
       </c>
       <c r="C65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D65" t="b">
         <v>0</v>
@@ -4402,7 +4408,7 @@
         <v>135</v>
       </c>
       <c r="C66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -4455,7 +4461,7 @@
         <v>137</v>
       </c>
       <c r="C67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D67" t="b">
         <v>0</v>
@@ -4490,7 +4496,7 @@
         <v>139</v>
       </c>
       <c r="C68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -4525,7 +4531,7 @@
         <v>141</v>
       </c>
       <c r="C69" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D69" t="b">
         <v>0</v>
@@ -4877,7 +4883,7 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B80" t="s">
         <v>195</v>
@@ -4885,7 +4891,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="B81" t="s">
         <v>196</v>
@@ -4893,10 +4899,18 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B82" t="s">
-        <v>200</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>211</v>
+      </c>
+      <c r="B83" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor data views from R functions to SQL database views
- Remove 10 R prep_view_* functions that built queries dynamically
- Add 12 SQL view definition files for database-side view creation
- Update modules to query pre-built database views directly
- Inline action item field mappings in module_action_item_tracking
- Simplify data_viewer module by removing df_view_meta dependency
</commit_message>
<xml_diff>
--- a/inputs/field and function mapping tables/df_views.xlsx
+++ b/inputs/field and function mapping tables/df_views.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotianaturetrust-my.sharepoint.com/personal/dominic_nsnt_ca/Documents/Documents/R Shiny/natureProps/inputs/field and function mapping tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="543" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB999478-2925-447F-8130-FA7654D6AD5E}"/>
+  <xr:revisionPtr revIDLastSave="545" documentId="8_{21D50595-6199-4E7F-94AC-CF188600A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11C8FB71-5CA4-4A2D-B0B9-BA45632FF1A3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
+    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{C915C129-1C36-402F-9A2F-BBF5BA1614C2}"/>
   </bookViews>
   <sheets>
     <sheet name="names" sheetId="1" r:id="rId1"/>
@@ -1544,8 +1544,8 @@
   <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>